<commit_message>
Excel Updated - ExecutionFlag added
</commit_message>
<xml_diff>
--- a/src/test/resources/inputData.xlsx
+++ b/src/test/resources/inputData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeyalakshmi\Jeya-API-Testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7995316E-C4F6-45E2-BE96-DEAF56157282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AE191F-E5DE-4E5E-B88A-E32EB504924D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DF0460C8-0C36-4F7A-B9C3-0EDAEEEC780A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>firstName</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Mani</t>
+  </si>
+  <si>
+    <t>Sno</t>
+  </si>
+  <si>
+    <t>ExecutionFlag</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -444,170 +456,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896E320E-C28D-445A-9307-184E4AD86305}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>101</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>11</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>78</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="b">
+      <c r="J2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>102</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>90</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="b">
+      <c r="J3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>103</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>12</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>56</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="b">
+      <c r="J4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>104</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>11</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>98</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="b">
+      <c r="J5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>105</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>88</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="b">
+      <c r="J6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>